<commit_message>
last updated date missing feature added
</commit_message>
<xml_diff>
--- a/assets/contacts_2.xlsx
+++ b/assets/contacts_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DE4808-BDD7-0944-9881-13FEA575A997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1ADA0-7E62-E94A-B40A-47E766BBA07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="15580" windowHeight="14900" xr2:uid="{70F11729-D218-AD4C-872F-E5D9D039EAC8}"/>
   </bookViews>
@@ -34,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>Rohit</t>
+  </si>
   <si>
     <t>Incidetns</t>
   </si>
@@ -54,26 +57,29 @@
     <t>Incidetn 2</t>
   </si>
   <si>
-    <t>Something 1</t>
-  </si>
-  <si>
-    <t>Something 2</t>
-  </si>
-  <si>
-    <t>Thifafa 1</t>
-  </si>
-  <si>
     <t>hello 1</t>
   </si>
   <si>
     <t>hello 2</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Last updated date</t>
+  </si>
+  <si>
+    <t>Rujuta</t>
+  </si>
+  <si>
+    <t>fsda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +94,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,9 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,54 +443,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4C8DD1-F9E7-CA42-B705-EB0E62F8096F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45111</v>
+      </c>
+      <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" s="2">
+        <v>45111</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>